<commit_message>
update 1 sept 2023
</commit_message>
<xml_diff>
--- a/excel/lorem.xlsx
+++ b/excel/lorem.xlsx
@@ -510,164 +510,164 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="2" min="2" width="11"/>
-    <col customWidth="true" max="3" min="3" width="5"/>
-    <col customWidth="true" max="4" min="4" width="27"/>
-    <col customWidth="true" max="5" min="5" width="12"/>
+    <col customWidth="true" max="1" min="1" width="11"/>
+    <col customWidth="true" max="2" min="2" width="5"/>
+    <col customWidth="true" max="3" min="3" width="27"/>
+    <col customWidth="true" max="4" min="4" width="12"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="4" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>